<commit_message>
Di edit Ho hendy 06 maret 2024
</commit_message>
<xml_diff>
--- a/Excel/Perdin.xlsx
+++ b/Excel/Perdin.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KATALON\Perjalanan Dinas\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ho.hendy\git\New-MySystem-Perdin-\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Master Biaya" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet2" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="200">
   <si>
     <t>Tipe Pengajuan</t>
   </si>
@@ -620,13 +620,22 @@
   </si>
   <si>
     <t>&gt; 16</t>
+  </si>
+  <si>
+    <t>Use</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -952,7 +961,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
@@ -965,7 +974,7 @@
     <col min="9" max="9" width="11.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -994,7 +1003,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>173</v>
       </c>
@@ -1079,87 +1088,87 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="37.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1">
       <c r="A14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1">
       <c r="A15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1177,167 +1186,167 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="36.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1">
       <c r="A14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1">
       <c r="A15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1">
       <c r="A16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1">
       <c r="A29" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1">
       <c r="A30" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1">
       <c r="A31" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -1355,562 +1364,562 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1">
       <c r="A14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1">
       <c r="A15" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1">
       <c r="A16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1">
       <c r="A29" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1">
       <c r="A30" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1">
       <c r="A31" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1">
       <c r="A32" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1">
       <c r="A33" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1">
       <c r="A34" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1">
       <c r="A35" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1">
       <c r="A36" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1">
       <c r="A37" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1">
       <c r="A38" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1">
       <c r="A39" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1">
       <c r="A40" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1">
       <c r="A41" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1">
       <c r="A42" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1">
       <c r="A43" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1">
       <c r="A44" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1">
       <c r="A45" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1">
       <c r="A46" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1">
       <c r="A47" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1">
       <c r="A48" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1">
       <c r="A49" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1">
       <c r="A50" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1">
       <c r="A51" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1">
       <c r="A52" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1">
       <c r="A53" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1">
       <c r="A54" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1">
       <c r="A55" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1">
       <c r="A56" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1">
       <c r="A57" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1">
       <c r="A58" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1">
       <c r="A59" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1">
       <c r="A60" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1">
       <c r="A61" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1">
       <c r="A62" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1">
       <c r="A63" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1">
       <c r="A64" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1">
       <c r="A65" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1">
       <c r="A66" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1">
       <c r="A67" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1">
       <c r="A68" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1">
       <c r="A69" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1">
       <c r="A70" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1">
       <c r="A71" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1">
       <c r="A72" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1">
       <c r="A73" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1">
       <c r="A74" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1">
       <c r="A75" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1">
       <c r="A76" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1">
       <c r="A77" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1">
       <c r="A78" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1">
       <c r="A79" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1">
       <c r="A80" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1">
       <c r="A81" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1">
       <c r="A82" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1">
       <c r="A83" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1">
       <c r="A84" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1">
       <c r="A85" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1">
       <c r="A86" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1">
       <c r="A87" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1">
       <c r="A88" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1">
       <c r="A89" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:1">
       <c r="A90" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1">
       <c r="A91" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1">
       <c r="A92" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1">
       <c r="A93" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1">
       <c r="A94" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1">
       <c r="A95" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1">
       <c r="A96" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1">
       <c r="A97" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1">
       <c r="A98" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1">
       <c r="A99" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1">
       <c r="A100" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1">
       <c r="A101" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1">
       <c r="A102" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1">
       <c r="A103" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1">
       <c r="A104" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:1">
       <c r="A105" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:1">
       <c r="A106" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:1">
       <c r="A107" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:1">
       <c r="A108" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:1">
       <c r="A109" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:1">
       <c r="A110" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:1">
       <c r="A111" t="s">
         <v>171</v>
       </c>
@@ -1922,103 +1931,154 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>175</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>176</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>177</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>179</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>180</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>194</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>185</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" t="s">
         <v>174</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>1000</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>178</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>181</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>185</v>
       </c>
-      <c r="H2" t="s">
-        <v>186</v>
-      </c>
       <c r="I2" t="s">
+        <v>187</v>
+      </c>
+      <c r="J2" t="s">
         <v>196</v>
       </c>
     </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>1000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>181</v>
+      </c>
+      <c r="H3" t="s">
+        <v>184</v>
+      </c>
+      <c r="I3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="F6" s="1"/>
+    </row>
   </sheetData>
-  <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2">
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6">
       <formula1>"Luar Negeri,Dalam Negeri,Luar Kota,Dalam Kota"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6">
       <formula1>"Transportasi,Uang Makan,Hotel"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6">
       <formula1>"1500,1000"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6">
       <formula1>"Iya,Tidak"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F6">
       <formula1>"100%,75%,0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G6">
       <formula1>"Aktif,Tidak Aktif"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J6">
       <formula1>"&gt; 16,&gt;= 12 &lt;= 16,&lt; 12"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A6">
+      <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2030,13 +2090,13 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>G2</xm:sqref>
+          <xm:sqref>H2:H6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet2!$B$4:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H2</xm:sqref>
+          <xm:sqref>I2:I6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2053,27 +2113,27 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>185</v>
       </c>
@@ -2087,27 +2147,27 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>193</v>
       </c>

</xml_diff>